<commit_message>
Membuat fungsi search data Penduduk
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23256" windowHeight="9504"/>
+    <workbookView windowWidth="21000" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>Data Penduduk</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Tempat, Tgl Lahir</t>
+  </si>
+  <si>
+    <t>Umur</t>
   </si>
   <si>
     <t xml:space="preserve">Alamat </t>
@@ -180,8 +183,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -201,13 +204,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -217,6 +214,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -230,6 +235,76 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -238,15 +313,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -254,30 +320,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -285,44 +327,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -330,9 +334,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -347,187 +350,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,24 +546,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -576,6 +566,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,15 +603,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -628,20 +618,33 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -659,130 +662,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1107,10 +1110,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1133,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1191,8 +1194,11 @@
       <c r="S3" t="s">
         <v>19</v>
       </c>
+      <c r="T3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>5120624252</v>
       </c>
@@ -1200,31 +1206,31 @@
         <v>5342783948</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="G4">
+      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
         <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s">
         <v>27</v>
@@ -1250,8 +1256,11 @@
       <c r="S4" t="s">
         <v>34</v>
       </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>5242533839</v>
       </c>
@@ -1259,58 +1268,61 @@
         <v>8666494040</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5">
         <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
       </c>
       <c r="I5" t="s">
         <v>38</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="L5" t="s">
         <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="N5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="O5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="Q5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="R5" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="S5" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="T5" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>5363738390</v>
       </c>
@@ -1318,22 +1330,22 @@
         <v>5647484901</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6">
         <v>7</v>
-      </c>
-      <c r="H6" t="s">
-        <v>45</v>
       </c>
       <c r="I6" t="s">
         <v>46</v>
@@ -1342,31 +1354,34 @@
         <v>47</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
         <v>27</v>
       </c>
       <c r="M6" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="N6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O6" t="s">
         <v>49</v>
       </c>
       <c r="P6" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="Q6" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="R6" t="s">
         <v>51</v>
       </c>
       <c r="S6" t="s">
         <v>52</v>
+      </c>
+      <c r="T6" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>